<commit_message>
BP-359 Bank excel statemenst upload
</commit_message>
<xml_diff>
--- a/src/test/resources/files/Reconciliation.xlsx
+++ b/src/test/resources/files/Reconciliation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2490C8E3-8163-4891-8837-1839BA72675F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A2E2F5-C295-402C-BA89-9B07F6A9C40C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="18000" windowHeight="9612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TRN_REF_NO</t>
   </si>
@@ -50,6 +50,21 @@
   </si>
   <si>
     <t>REF_NO</t>
+  </si>
+  <si>
+    <t>199999</t>
+  </si>
+  <si>
+    <t>288888</t>
+  </si>
+  <si>
+    <t>388888</t>
+  </si>
+  <si>
+    <t>488888</t>
+  </si>
+  <si>
+    <t>588888</t>
   </si>
 </sst>
 </file>
@@ -85,9 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,17 +388,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,92 +415,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>220477960</v>
       </c>
-      <c r="B2">
-        <v>99999</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>44411</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>5500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>220449200</v>
       </c>
-      <c r="B3">
-        <v>88888</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>44411</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>220558882</v>
       </c>
-      <c r="B4">
-        <v>88888</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1">
         <v>44411</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>220447776</v>
       </c>
-      <c r="B5">
-        <v>88888</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>44411</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>2500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>220430412</v>
       </c>
-      <c r="B6">
-        <v>88888</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>44411</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>300.45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>